<commit_message>
CSV/Excel arreglado y Modelo KNN
</commit_message>
<xml_diff>
--- a/PC1/BreastCancerDataSet_LimpiezaCompletada.xlsx
+++ b/PC1/BreastCancerDataSet_LimpiezaCompletada.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3672F9B1-7711-46EC-9BFD-B3CBFEF7BFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CB8858-6F1C-48C9-91B2-A8E9D62C93B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{500F79F8-CBFF-4C20-984A-7AA980DC530A}"/>
   </bookViews>
@@ -180,7 +180,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB396CC2-B965-4E23-BA88-B490C870CF4D}" name="DataSet_SinDatosPerdidos" displayName="DataSet_SinDatosPerdidos" ref="A1:J278" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:J278" xr:uid="{FB396CC2-B965-4E23-BA88-B490C870CF4D}"/>
+  <autoFilter ref="A1:J278" xr:uid="{FB396CC2-B965-4E23-BA88-B490C870CF4D}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{18BF7AB6-D7F3-438D-9E16-191DC60E399C}" uniqueName="1" name="Class" queryTableFieldId="1" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{15A46732-F818-4D4D-86A2-34DA5B21B309}" uniqueName="2" name="age" queryTableFieldId="2" dataDxfId="7"/>
@@ -496,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F3ED86-4F9B-40C6-8F0F-2E665781AF2A}">
   <dimension ref="A1:J278"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A264" workbookViewId="0">
+      <selection activeCell="B280" sqref="B280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,9 +552,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -578,9 +584,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
@@ -610,9 +616,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -642,9 +648,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -674,9 +680,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
@@ -706,9 +712,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>
@@ -738,9 +744,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="1">
         <v>4</v>
@@ -770,9 +776,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" s="1">
         <v>5</v>
@@ -802,9 +808,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
@@ -834,9 +840,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
@@ -866,9 +872,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" s="1">
         <v>3</v>
@@ -898,9 +904,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" s="1">
         <v>4</v>
@@ -930,9 +936,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" s="1">
         <v>5</v>
@@ -962,9 +968,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
@@ -994,9 +1000,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
@@ -1026,9 +1032,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" s="1">
         <v>5</v>
@@ -1058,9 +1064,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
@@ -1090,9 +1096,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" s="1">
         <v>4</v>
@@ -1122,9 +1128,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" s="1">
         <v>5</v>
@@ -1154,9 +1160,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" s="1">
         <v>4</v>
@@ -1186,9 +1192,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" s="1">
         <v>4</v>
@@ -1218,9 +1224,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" s="1">
         <v>5</v>
@@ -1250,9 +1256,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" s="1">
         <v>2</v>
@@ -1282,9 +1288,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" s="1">
         <v>4</v>
@@ -1314,9 +1320,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" s="1">
         <v>4</v>
@@ -1346,9 +1352,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" s="1">
         <v>3</v>
@@ -1378,9 +1384,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" s="1">
         <v>4</v>
@@ -1410,9 +1416,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" s="1">
         <v>5</v>
@@ -1442,9 +1448,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" s="1">
         <v>3</v>
@@ -1474,9 +1480,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B31" s="1">
         <v>5</v>
@@ -1506,9 +1512,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" s="1">
         <v>4</v>
@@ -1538,9 +1544,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" s="1">
         <v>4</v>
@@ -1570,9 +1576,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" s="1">
         <v>4</v>
@@ -1602,9 +1608,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" s="1">
         <v>4</v>
@@ -1634,9 +1640,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36" s="1">
         <v>4</v>
@@ -1666,9 +1672,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" s="1">
         <v>2</v>
@@ -1698,9 +1704,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B38" s="1">
         <v>4</v>
@@ -1730,9 +1736,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39" s="1">
         <v>4</v>
@@ -1762,9 +1768,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40" s="1">
         <v>3</v>
@@ -1794,9 +1800,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B41" s="1">
         <v>3</v>
@@ -1826,9 +1832,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B42" s="1">
         <v>4</v>
@@ -1858,9 +1864,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B43" s="1">
         <v>5</v>
@@ -1890,9 +1896,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B44" s="1">
         <v>5</v>
@@ -1922,9 +1928,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B45" s="1">
         <v>3</v>
@@ -1954,9 +1960,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B46" s="1">
         <v>4</v>
@@ -1986,9 +1992,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B47" s="1">
         <v>4</v>
@@ -2018,9 +2024,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B48" s="1">
         <v>3</v>
@@ -2050,9 +2056,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B49" s="1">
         <v>4</v>
@@ -2082,9 +2088,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B50" s="1">
         <v>3</v>
@@ -2114,9 +2120,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B51" s="1">
         <v>3</v>
@@ -2146,9 +2152,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B52" s="1">
         <v>4</v>
@@ -2178,9 +2184,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B53" s="1">
         <v>2</v>
@@ -2210,9 +2216,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B54" s="1">
         <v>4</v>
@@ -2242,9 +2248,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B55" s="1">
         <v>6</v>
@@ -2274,9 +2280,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B56" s="1">
         <v>6</v>
@@ -2306,9 +2312,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B57" s="1">
         <v>6</v>
@@ -2338,9 +2344,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B58" s="1">
         <v>4</v>
@@ -2370,9 +2376,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B59" s="1">
         <v>4</v>
@@ -2402,9 +2408,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B60" s="1">
         <v>5</v>
@@ -2434,9 +2440,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B61" s="1">
         <v>5</v>
@@ -2466,9 +2472,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B62" s="1">
         <v>3</v>
@@ -2498,9 +2504,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B63" s="1">
         <v>3</v>
@@ -2530,9 +2536,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B64" s="1">
         <v>4</v>
@@ -2562,9 +2568,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B65" s="1">
         <v>1</v>
@@ -2594,9 +2600,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B66" s="1">
         <v>3</v>
@@ -2626,9 +2632,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B67" s="1">
         <v>3</v>
@@ -2658,9 +2664,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B68" s="1">
         <v>3</v>
@@ -2690,9 +2696,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B69" s="1">
         <v>4</v>
@@ -2722,9 +2728,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B70" s="1">
         <v>4</v>
@@ -2754,9 +2760,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B71" s="1">
         <v>5</v>
@@ -2786,9 +2792,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B72" s="1">
         <v>5</v>
@@ -2818,9 +2824,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B73" s="1">
         <v>3</v>
@@ -2850,9 +2856,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B74" s="1">
         <v>5</v>
@@ -2882,9 +2888,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B75" s="1">
         <v>4</v>
@@ -2914,9 +2920,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B76" s="1">
         <v>2</v>
@@ -2946,9 +2952,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B77" s="1">
         <v>4</v>
@@ -2978,9 +2984,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B78" s="1">
         <v>4</v>
@@ -3010,9 +3016,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B79" s="1">
         <v>2</v>
@@ -3042,9 +3048,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B80" s="1">
         <v>4</v>
@@ -3074,9 +3080,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B81" s="1">
         <v>3</v>
@@ -3106,9 +3112,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B82" s="1">
         <v>4</v>
@@ -3138,9 +3144,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B83" s="1">
         <v>5</v>
@@ -3170,9 +3176,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B84" s="1">
         <v>5</v>
@@ -3202,9 +3208,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B85" s="1">
         <v>4</v>
@@ -3234,9 +3240,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B86" s="1">
         <v>3</v>
@@ -3266,9 +3272,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B87" s="1">
         <v>4</v>
@@ -3298,9 +3304,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B88" s="1">
         <v>5</v>
@@ -3330,9 +3336,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B89" s="1">
         <v>6</v>
@@ -3362,9 +3368,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B90" s="1">
         <v>4</v>
@@ -3394,9 +3400,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B91" s="1">
         <v>3</v>
@@ -3426,9 +3432,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B92" s="1">
         <v>2</v>
@@ -3458,9 +3464,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B93" s="1">
         <v>4</v>
@@ -3490,9 +3496,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B94" s="1">
         <v>4</v>
@@ -3522,9 +3528,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B95" s="1">
         <v>5</v>
@@ -3554,9 +3560,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B96" s="1">
         <v>4</v>
@@ -3586,9 +3592,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B97" s="1">
         <v>3</v>
@@ -3618,9 +3624,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B98" s="1">
         <v>5</v>
@@ -3650,9 +3656,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B99" s="1">
         <v>5</v>
@@ -3682,9 +3688,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B100" s="1">
         <v>3</v>
@@ -3714,9 +3720,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B101" s="1">
         <v>2</v>
@@ -3746,9 +3752,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B102" s="1">
         <v>3</v>
@@ -3778,9 +3784,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B103" s="1">
         <v>4</v>
@@ -3810,9 +3816,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B104" s="1">
         <v>4</v>
@@ -3842,9 +3848,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B105" s="1">
         <v>3</v>
@@ -3874,9 +3880,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B106" s="1">
         <v>3</v>
@@ -3906,9 +3912,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B107" s="1">
         <v>3</v>
@@ -3938,9 +3944,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B108" s="1">
         <v>3</v>
@@ -3970,9 +3976,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B109" s="1">
         <v>2</v>
@@ -4002,9 +4008,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B110" s="1">
         <v>3</v>
@@ -4034,9 +4040,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B111" s="1">
         <v>5</v>
@@ -4066,9 +4072,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B112" s="1">
         <v>4</v>
@@ -4098,9 +4104,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B113" s="1">
         <v>4</v>
@@ -4130,9 +4136,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B114" s="1">
         <v>3</v>
@@ -4162,9 +4168,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B115" s="1">
         <v>3</v>
@@ -4194,9 +4200,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B116" s="1">
         <v>3</v>
@@ -4226,9 +4232,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B117" s="1">
         <v>4</v>
@@ -4258,9 +4264,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B118" s="1">
         <v>2</v>
@@ -4290,9 +4296,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B119" s="1">
         <v>3</v>
@@ -4322,9 +4328,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B120" s="1">
         <v>2</v>
@@ -4354,9 +4360,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B121" s="1">
         <v>5</v>
@@ -4386,9 +4392,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B122" s="1">
         <v>5</v>
@@ -4418,9 +4424,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B123" s="1">
         <v>4</v>
@@ -4450,9 +4456,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B124" s="1">
         <v>4</v>
@@ -4482,9 +4488,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B125" s="1">
         <v>4</v>
@@ -4514,9 +4520,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B126" s="1">
         <v>5</v>
@@ -4546,9 +4552,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B127" s="1">
         <v>6</v>
@@ -4578,9 +4584,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B128" s="1">
         <v>2</v>
@@ -4610,9 +4616,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B129" s="1">
         <v>2</v>
@@ -4642,9 +4648,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B130" s="1">
         <v>4</v>
@@ -4674,9 +4680,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B131" s="1">
         <v>3</v>
@@ -4706,9 +4712,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B132" s="1">
         <v>3</v>
@@ -4738,9 +4744,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B133" s="1">
         <v>3</v>
@@ -4770,9 +4776,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B134" s="1">
         <v>3</v>
@@ -4802,9 +4808,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B135" s="1">
         <v>4</v>
@@ -4834,9 +4840,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B136" s="1">
         <v>5</v>
@@ -4866,9 +4872,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B137" s="1">
         <v>2</v>
@@ -4898,9 +4904,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B138" s="1">
         <v>2</v>
@@ -4930,9 +4936,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B139" s="1">
         <v>3</v>
@@ -4962,9 +4968,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B140" s="1">
         <v>2</v>
@@ -4994,9 +5000,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B141" s="1">
         <v>3</v>
@@ -5026,9 +5032,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B142" s="1">
         <v>4</v>
@@ -5058,9 +5064,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B143" s="1">
         <v>4</v>
@@ -5090,9 +5096,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B144" s="1">
         <v>5</v>
@@ -5122,9 +5128,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B145" s="1">
         <v>3</v>
@@ -5154,9 +5160,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B146" s="1">
         <v>5</v>
@@ -5186,9 +5192,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B147" s="1">
         <v>5</v>
@@ -5218,9 +5224,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B148" s="1">
         <v>4</v>
@@ -5250,9 +5256,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B149" s="1">
         <v>2</v>
@@ -5282,9 +5288,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B150" s="1">
         <v>4</v>
@@ -5314,9 +5320,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B151" s="1">
         <v>4</v>
@@ -5346,9 +5352,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B152" s="1">
         <v>5</v>
@@ -5378,9 +5384,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B153" s="1">
         <v>4</v>
@@ -5410,9 +5416,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B154" s="1">
         <v>5</v>
@@ -5442,9 +5448,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B155" s="1">
         <v>2</v>
@@ -5474,9 +5480,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B156" s="1">
         <v>5</v>
@@ -5506,9 +5512,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B157" s="1">
         <v>4</v>
@@ -5538,9 +5544,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B158" s="1">
         <v>4</v>
@@ -5570,9 +5576,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B159" s="1">
         <v>4</v>
@@ -5602,9 +5608,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B160" s="1">
         <v>3</v>
@@ -5634,9 +5640,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B161" s="1">
         <v>3</v>
@@ -5666,9 +5672,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B162" s="1">
         <v>3</v>
@@ -5698,9 +5704,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B163" s="1">
         <v>5</v>
@@ -5730,9 +5736,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B164" s="1">
         <v>3</v>
@@ -5762,9 +5768,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B165" s="1">
         <v>3</v>
@@ -5794,9 +5800,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B166" s="1">
         <v>3</v>
@@ -5826,9 +5832,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B167" s="1">
         <v>4</v>
@@ -5858,9 +5864,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B168" s="1">
         <v>3</v>
@@ -5890,9 +5896,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B169" s="1">
         <v>2</v>
@@ -5922,9 +5928,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B170" s="1">
         <v>2</v>
@@ -5954,9 +5960,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B171" s="1">
         <v>5</v>
@@ -5986,9 +5992,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B172" s="1">
         <v>4</v>
@@ -6018,9 +6024,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B173" s="1">
         <v>4</v>
@@ -6050,9 +6056,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B174" s="1">
         <v>3</v>
@@ -6082,9 +6088,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B175" s="1">
         <v>3</v>
@@ -6114,9 +6120,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B176" s="1">
         <v>5</v>
@@ -6146,9 +6152,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B177" s="1">
         <v>4</v>
@@ -6178,9 +6184,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B178" s="1">
         <v>3</v>
@@ -6210,9 +6216,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B179" s="1">
         <v>3</v>
@@ -6242,9 +6248,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B180" s="1">
         <v>3</v>
@@ -6274,9 +6280,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B181" s="1">
         <v>3</v>
@@ -6306,9 +6312,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B182" s="1">
         <v>3</v>
@@ -6338,9 +6344,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B183" s="1">
         <v>4</v>
@@ -6370,9 +6376,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B184" s="1">
         <v>5</v>
@@ -6402,9 +6408,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B185" s="1">
         <v>3</v>
@@ -6434,9 +6440,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B186" s="1">
         <v>4</v>
@@ -6466,9 +6472,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B187" s="1">
         <v>3</v>
@@ -6498,9 +6504,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B188" s="1">
         <v>3</v>
@@ -6530,9 +6536,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B189" s="1">
         <v>4</v>
@@ -6562,9 +6568,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B190" s="1">
         <v>2</v>
@@ -6594,9 +6600,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B191" s="1">
         <v>4</v>
@@ -6626,9 +6632,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B192" s="1">
         <v>4</v>
@@ -6658,9 +6664,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B193" s="1">
         <v>4</v>
@@ -6690,9 +6696,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B194" s="1">
         <v>3</v>
@@ -6722,9 +6728,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B195" s="1">
         <v>4</v>
@@ -6754,9 +6760,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B196" s="1">
         <v>4</v>
@@ -6786,9 +6792,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B197" s="1">
         <v>5</v>
@@ -6820,7 +6826,7 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B198" s="1">
         <v>4</v>
@@ -6852,7 +6858,7 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B199" s="1">
         <v>3</v>
@@ -6884,7 +6890,7 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B200" s="1">
         <v>4</v>
@@ -6916,7 +6922,7 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B201" s="1">
         <v>4</v>
@@ -6948,7 +6954,7 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B202" s="1">
         <v>2</v>
@@ -6980,7 +6986,7 @@
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B203" s="1">
         <v>4</v>
@@ -7012,7 +7018,7 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B204" s="1">
         <v>4</v>
@@ -7044,7 +7050,7 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B205" s="1">
         <v>3</v>
@@ -7076,7 +7082,7 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B206" s="1">
         <v>3</v>
@@ -7108,7 +7114,7 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B207" s="1">
         <v>4</v>
@@ -7140,7 +7146,7 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B208" s="1">
         <v>3</v>
@@ -7172,7 +7178,7 @@
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B209" s="1">
         <v>4</v>
@@ -7204,7 +7210,7 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B210" s="1">
         <v>5</v>
@@ -7236,7 +7242,7 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B211" s="1">
         <v>3</v>
@@ -7268,7 +7274,7 @@
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B212" s="1">
         <v>4</v>
@@ -7300,7 +7306,7 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B213" s="1">
         <v>3</v>
@@ -7332,7 +7338,7 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B214" s="1">
         <v>5</v>
@@ -7364,7 +7370,7 @@
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B215" s="1">
         <v>2</v>
@@ -7396,7 +7402,7 @@
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B216" s="1">
         <v>3</v>
@@ -7428,7 +7434,7 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B217" s="1">
         <v>2</v>
@@ -7460,7 +7466,7 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B218" s="1">
         <v>5</v>
@@ -7492,7 +7498,7 @@
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B219" s="1">
         <v>5</v>
@@ -7524,7 +7530,7 @@
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B220" s="1">
         <v>2</v>
@@ -7556,7 +7562,7 @@
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B221" s="1">
         <v>3</v>
@@ -7588,7 +7594,7 @@
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B222" s="1">
         <v>3</v>
@@ -7620,7 +7626,7 @@
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B223" s="1">
         <v>4</v>
@@ -7652,7 +7658,7 @@
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B224" s="1">
         <v>5</v>
@@ -7684,7 +7690,7 @@
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B225" s="1">
         <v>5</v>
@@ -7716,7 +7722,7 @@
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B226" s="1">
         <v>4</v>
@@ -7748,7 +7754,7 @@
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B227" s="1">
         <v>3</v>
@@ -7780,7 +7786,7 @@
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B228" s="1">
         <v>2</v>
@@ -7812,7 +7818,7 @@
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B229" s="1">
         <v>5</v>
@@ -7844,7 +7850,7 @@
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B230" s="1">
         <v>4</v>
@@ -7876,7 +7882,7 @@
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B231" s="1">
         <v>3</v>
@@ -7908,7 +7914,7 @@
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B232" s="1">
         <v>3</v>
@@ -7940,7 +7946,7 @@
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B233" s="1">
         <v>2</v>
@@ -7972,7 +7978,7 @@
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B234" s="1">
         <v>3</v>
@@ -8004,7 +8010,7 @@
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B235" s="1">
         <v>5</v>
@@ -8036,7 +8042,7 @@
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B236" s="1">
         <v>3</v>
@@ -8068,7 +8074,7 @@
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B237" s="1">
         <v>4</v>
@@ -8100,7 +8106,7 @@
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B238" s="1">
         <v>4</v>
@@ -8132,7 +8138,7 @@
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B239" s="1">
         <v>3</v>
@@ -8164,7 +8170,7 @@
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B240" s="1">
         <v>2</v>
@@ -8196,7 +8202,7 @@
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B241" s="1">
         <v>2</v>
@@ -8228,7 +8234,7 @@
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B242" s="1">
         <v>4</v>
@@ -8260,7 +8266,7 @@
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B243" s="1">
         <v>5</v>
@@ -8292,7 +8298,7 @@
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B244" s="1">
         <v>2</v>
@@ -8324,7 +8330,7 @@
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B245" s="1">
         <v>3</v>
@@ -8356,7 +8362,7 @@
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B246" s="1">
         <v>3</v>
@@ -8388,7 +8394,7 @@
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B247" s="1">
         <v>2</v>
@@ -8420,7 +8426,7 @@
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B248" s="1">
         <v>5</v>
@@ -8452,7 +8458,7 @@
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B249" s="1">
         <v>3</v>
@@ -8484,7 +8490,7 @@
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B250" s="1">
         <v>3</v>
@@ -8516,7 +8522,7 @@
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B251" s="1">
         <v>3</v>
@@ -8548,7 +8554,7 @@
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B252" s="1">
         <v>3</v>
@@ -8580,7 +8586,7 @@
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B253" s="1">
         <v>4</v>
@@ -8612,7 +8618,7 @@
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B254" s="1">
         <v>4</v>
@@ -8644,7 +8650,7 @@
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B255" s="1">
         <v>5</v>
@@ -8676,7 +8682,7 @@
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B256" s="1">
         <v>3</v>
@@ -8708,7 +8714,7 @@
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B257" s="1">
         <v>5</v>
@@ -8740,7 +8746,7 @@
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B258" s="1">
         <v>2</v>
@@ -8772,7 +8778,7 @@
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B259" s="1">
         <v>3</v>
@@ -8804,7 +8810,7 @@
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B260" s="1">
         <v>5</v>
@@ -8836,7 +8842,7 @@
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B261" s="1">
         <v>2</v>
@@ -8868,7 +8874,7 @@
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B262" s="1">
         <v>3</v>
@@ -8900,7 +8906,7 @@
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B263" s="1">
         <v>4</v>
@@ -8932,7 +8938,7 @@
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B264" s="1">
         <v>4</v>
@@ -8964,7 +8970,7 @@
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B265" s="1">
         <v>3</v>
@@ -8996,7 +9002,7 @@
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B266" s="1">
         <v>5</v>
@@ -9028,7 +9034,7 @@
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B267" s="1">
         <v>5</v>
@@ -9060,7 +9066,7 @@
     </row>
     <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B268" s="1">
         <v>3</v>
@@ -9092,7 +9098,7 @@
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B269" s="1">
         <v>2</v>
@@ -9124,7 +9130,7 @@
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B270" s="1">
         <v>5</v>
@@ -9156,7 +9162,7 @@
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B271" s="1">
         <v>4</v>
@@ -9188,7 +9194,7 @@
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B272" s="1">
         <v>4</v>
@@ -9220,7 +9226,7 @@
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B273" s="1">
         <v>4</v>
@@ -9252,7 +9258,7 @@
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B274" s="1">
         <v>2</v>
@@ -9284,7 +9290,7 @@
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B275" s="1">
         <v>2</v>
@@ -9316,7 +9322,7 @@
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B276" s="1">
         <v>5</v>
@@ -9348,7 +9354,7 @@
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B277" s="1">
         <v>3</v>
@@ -9380,7 +9386,7 @@
     </row>
     <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B278" s="1">
         <v>4</v>

</xml_diff>